<commit_message>
Pulled data to new sheets
</commit_message>
<xml_diff>
--- a/WT Survey Data/Questions.xlsx
+++ b/WT Survey Data/Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bret\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwmcs\OneDrive\Documents\GitHub\spring-2018-final-projects-bretbryan-wt\WT Survey Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A46C521-8514-4322-9332-251A70E831BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{4A46C521-8514-4322-9332-251A70E831BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{7C8B4EE5-684F-4B2C-BDF9-D8997EC7EC1E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{DF3E8A89-828C-4955-9B05-231EFFB47096}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6948" xr2:uid="{DF3E8A89-828C-4955-9B05-231EFFB47096}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -928,12 +928,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -948,13 +954,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1273,18 +1282,19 @@
   <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="50.7109375" style="1"/>
-    <col min="3" max="3" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="50.7109375" style="1"/>
+    <col min="1" max="2" width="50.6640625" style="1"/>
+    <col min="3" max="3" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="50.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1308,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1309,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1320,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1331,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1353,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1364,7 +1374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1437,7 +1447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1478,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1488,7 +1498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1508,7 +1518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1528,7 +1538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1548,7 +1558,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1565,7 +1575,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1590,7 +1600,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1601,7 +1611,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1612,7 +1622,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1623,7 +1633,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1637,7 +1647,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1654,7 +1664,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1671,7 +1681,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1685,7 +1695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1716,7 +1726,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1733,7 +1743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1747,7 +1757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
@@ -1758,7 +1768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1772,7 +1782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1783,7 +1793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1794,7 +1804,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1808,7 +1818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1825,7 +1835,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1836,7 +1846,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1847,7 +1857,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1875,7 +1885,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1892,7 +1902,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>50</v>
       </c>
@@ -1909,7 +1919,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1923,7 +1933,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>52</v>
       </c>
@@ -1934,7 +1944,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>55</v>
       </c>
@@ -1959,7 +1969,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>56</v>
       </c>
@@ -1970,7 +1980,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>57</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>58</v>
       </c>
@@ -2001,7 +2011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
@@ -2015,7 +2025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>60</v>
       </c>
@@ -2029,7 +2039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
@@ -2046,7 +2056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -2066,7 +2076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>63</v>
       </c>
@@ -2083,7 +2093,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>65</v>
       </c>
@@ -2094,7 +2104,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>66</v>
       </c>
@@ -2108,7 +2118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>67</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>68</v>
       </c>
@@ -2136,7 +2146,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>69</v>
       </c>
@@ -2150,7 +2160,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>70</v>
       </c>
@@ -2161,7 +2171,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>71</v>
       </c>
@@ -2175,7 +2185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>72</v>
       </c>
@@ -2189,7 +2199,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>73</v>
       </c>
@@ -2200,7 +2210,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
         <v>74</v>
       </c>
@@ -2211,7 +2221,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>75</v>
       </c>
@@ -2225,8 +2235,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
+    <row r="68" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B68" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2239,8 +2249,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="210" x14ac:dyDescent="0.25">
-      <c r="B69" s="1" t="s">
+    <row r="69" spans="2:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B69" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -2253,8 +2263,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="255" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
+    <row r="70" spans="2:6" ht="216" x14ac:dyDescent="0.3">
+      <c r="B70" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2267,8 +2277,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
+    <row r="71" spans="2:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B71" s="3" t="s">
         <v>79</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2278,7 +2288,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
@@ -2289,7 +2299,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>81</v>
       </c>
@@ -2303,7 +2313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
@@ -2317,7 +2327,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>83</v>
       </c>
@@ -2328,7 +2338,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>84</v>
       </c>
@@ -2342,7 +2352,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>85</v>
       </c>
@@ -2356,7 +2366,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>86</v>
       </c>
@@ -2373,7 +2383,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>87</v>
       </c>
@@ -2387,7 +2397,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>88</v>
       </c>
@@ -2398,7 +2408,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>89</v>
       </c>
@@ -2409,7 +2419,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>90</v>
       </c>
@@ -2420,7 +2430,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>91</v>
       </c>
@@ -2431,7 +2441,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>92</v>
       </c>
@@ -2448,7 +2458,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>93</v>
       </c>
@@ -2462,7 +2472,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
         <v>94</v>
       </c>
@@ -2473,7 +2483,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
         <v>95</v>
       </c>
@@ -2484,7 +2494,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>96</v>
       </c>
@@ -2498,7 +2508,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>97</v>
       </c>
@@ -2512,7 +2522,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
         <v>98</v>
       </c>
@@ -2526,7 +2536,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
         <v>99</v>
       </c>
@@ -2537,8 +2547,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
+    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -2548,24 +2559,27 @@
         <v>255</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3" t="s">
         <v>102</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
+    <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E95" s="1" t="s">
@@ -2575,7 +2589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>104</v>
       </c>
@@ -2589,7 +2603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>105</v>
       </c>
@@ -2600,7 +2614,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>62</v>
       </c>
@@ -2614,7 +2628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>63</v>
       </c>
@@ -2628,7 +2642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>65</v>
       </c>
@@ -2639,7 +2653,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>66</v>
       </c>
@@ -2647,7 +2661,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B102" s="1" t="s">
         <v>67</v>
       </c>
@@ -2655,7 +2669,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B103" s="1" t="s">
         <v>68</v>
       </c>
@@ -2663,7 +2677,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B104" s="1" t="s">
         <v>69</v>
       </c>
@@ -2674,7 +2688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
         <v>70</v>
       </c>
@@ -2685,7 +2699,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
         <v>71</v>
       </c>
@@ -2693,7 +2707,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
         <v>72</v>
       </c>
@@ -2704,7 +2718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>73</v>
       </c>
@@ -2715,7 +2729,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
         <v>74</v>
       </c>
@@ -2723,7 +2737,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B110" s="1" t="s">
         <v>75</v>
       </c>
@@ -2731,7 +2745,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>76</v>
       </c>
@@ -2739,7 +2753,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>77</v>
       </c>
@@ -2750,7 +2764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" s="1" t="s">
         <v>78</v>
       </c>
@@ -2761,7 +2775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="1" t="s">
         <v>79</v>
       </c>
@@ -2772,7 +2786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115" s="1" t="s">
         <v>80</v>
       </c>
@@ -2783,7 +2797,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>81</v>
       </c>
@@ -2791,7 +2805,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B117" s="1" t="s">
         <v>82</v>
       </c>
@@ -2799,7 +2813,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>83</v>
       </c>
@@ -2807,7 +2821,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>84</v>
       </c>
@@ -2815,7 +2829,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
         <v>85</v>
       </c>
@@ -2823,7 +2837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>86</v>
       </c>
@@ -2834,7 +2848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>87</v>
       </c>
@@ -2845,7 +2859,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="123" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B123" s="1" t="s">
         <v>88</v>
       </c>
@@ -2853,7 +2867,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B124" s="1" t="s">
         <v>89</v>
       </c>
@@ -2861,7 +2875,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125" s="1" t="s">
         <v>90</v>
       </c>
@@ -2869,7 +2883,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="126" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B126" s="1" t="s">
         <v>91</v>
       </c>
@@ -2880,7 +2894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B127" s="1" t="s">
         <v>92</v>
       </c>
@@ -2891,7 +2905,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B128" s="1" t="s">
         <v>93</v>
       </c>
@@ -2902,7 +2916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>94</v>
       </c>
@@ -2913,7 +2927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>95</v>
       </c>
@@ -2924,7 +2938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>96</v>
       </c>
@@ -2935,7 +2949,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>97</v>
       </c>
@@ -2943,7 +2957,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>98</v>
       </c>
@@ -2951,7 +2965,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>99</v>
       </c>
@@ -2959,7 +2973,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>100</v>
       </c>
@@ -2967,7 +2981,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B136" s="1" t="s">
         <v>101</v>
       </c>
@@ -2975,7 +2989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B137" s="1" t="s">
         <v>102</v>
       </c>
@@ -2986,7 +3000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B138" s="1" t="s">
         <v>103</v>
       </c>
@@ -2997,7 +3011,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>104</v>
       </c>
@@ -3008,17 +3022,17 @@
         <v>286</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F140" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F141" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E142" s="1" t="s">
         <v>293</v>
       </c>
@@ -3026,7 +3040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E143" s="1" t="s">
         <v>294</v>
       </c>
@@ -3034,7 +3048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E144" s="1" t="s">
         <v>295</v>
       </c>

</xml_diff>